<commit_message>
fix(excel): table columns init
</commit_message>
<xml_diff>
--- a/excel/db.xlsx
+++ b/excel/db.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="CONTACTS" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="USERS" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="USERS" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="CONTACTS" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,32 +425,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>FIRSTNAME</t>
+          <t>USERNAME</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>FIRSTNAME</t>
+          <t>PASSWORD</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>FIRSTNAME</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>FIRSTNAME</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>FIRSTNAME</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>FIRSTNAME</t>
+          <t>CREATE_AT</t>
         </is>
       </c>
     </row>
@@ -465,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,17 +461,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>USERNAME</t>
+          <t>FIRSTNAME</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>USERNAME</t>
+          <t>MIDDLENAME</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>USERNAME</t>
+          <t>LASTNAME</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>PHONE</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>EMAIL</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>COMMENT</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>CREATED_AT</t>
         </is>
       </c>
     </row>

</xml_diff>